<commit_message>
finished looking at PSME issues. Made rmd's for quhy and quar09
</commit_message>
<xml_diff>
--- a/PSME flags_wStatus 2024-02-12 .xlsx
+++ b/PSME flags_wStatus 2024-02-12 .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/edeegan_nps_gov/Documents/FFIqaqc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="11_1ED3C718C480BD8DCCCFE1C6C6240EC8918A27CD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D7007FD-2DA4-4F82-857D-B252D92C10D7}"/>
+  <xr:revisionPtr revIDLastSave="265" documentId="11_1ED3C718C480BD8DCCCFE1C6C6240EC8918A27CD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C642F0E-149D-464A-B3F3-5E4E0C312269}"/>
   <bookViews>
-    <workbookView xWindow="47910" yWindow="-15870" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47910" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PSME-01" sheetId="1" r:id="rId1"/>
@@ -3456,8 +3456,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3756,8 +3757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5774,7 +5775,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B120" t="s">
@@ -5815,7 +5816,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+      <c r="A124" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B124" t="s">
@@ -5832,7 +5833,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B125" t="s">
@@ -5899,7 +5900,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B130" t="s">
@@ -5965,7 +5966,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+      <c r="A136" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B136" t="s">
@@ -6656,7 +6657,7 @@
   <autoFilter ref="B1:B197" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8041,8 +8042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75:B82"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8079,7 +8080,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>206</v>
       </c>
       <c r="B3" t="s">
@@ -8096,7 +8097,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B4" t="s">
@@ -8113,7 +8114,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B5" t="s">
@@ -8130,7 +8131,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>209</v>
       </c>
       <c r="B6" t="s">
@@ -8147,7 +8148,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B7" t="s">
@@ -8987,7 +8988,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>261</v>
       </c>
       <c r="B58" t="s">
@@ -9004,7 +9005,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>262</v>
       </c>
       <c r="B59" t="s">
@@ -9021,7 +9022,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>263</v>
       </c>
       <c r="B60" t="s">
@@ -9290,7 +9291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B97" sqref="B97:B111"/>
     </sheetView>
   </sheetViews>

</xml_diff>